<commit_message>
Update control so ETC can accept a throttle input from the vector box
</commit_message>
<xml_diff>
--- a/matlab_code/etc_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/etc_benchTest/CANmailboxUsage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\etc_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493BD58B-8181-4532-8B41-98995E3A6477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F346C8CB-C84E-4B19-A504-AD2C4E3800B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Output</t>
+  </si>
+  <si>
+    <t>HI_VectorBox</t>
+  </si>
+  <si>
+    <t>Input</t>
   </si>
 </sst>
 </file>
@@ -369,7 +375,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,6 +512,12 @@
       <c r="B14">
         <v>11</v>
       </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15">

</xml_diff>

<commit_message>
Add in logging for motor control gains. Decrease time constant of deriative for the motor velocity calculation to make it more responsive.
</commit_message>
<xml_diff>
--- a/matlab_code/etc_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/etc_benchTest/CANmailboxUsage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\etc_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F346C8CB-C84E-4B19-A504-AD2C4E3800B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEBBC9C-BEAA-4675-80AC-E9CEC19D79C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -375,7 +375,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,6 +523,12 @@
       <c r="B15">
         <v>12</v>
       </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16">

</xml_diff>

<commit_message>
Add basic etc modes to the model
</commit_message>
<xml_diff>
--- a/matlab_code/etc_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/etc_benchTest/CANmailboxUsage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\etc_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEBBC9C-BEAA-4675-80AC-E9CEC19D79C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D32E32B-9904-4883-BBD4-078F53832004}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -39,9 +39,6 @@
     <t>HO_VectorBox/motorMeasurements</t>
   </si>
   <si>
-    <t>HO_VectorBox/motorControl</t>
-  </si>
-  <si>
     <t>CCP</t>
   </si>
   <si>
@@ -55,6 +52,15 @@
   </si>
   <si>
     <t>Input</t>
+  </si>
+  <si>
+    <t>HO_VectorBox/modes</t>
+  </si>
+  <si>
+    <t>HO_VectorBox/motorControlSlow</t>
+  </si>
+  <si>
+    <t>HO_VectorBox/motorControlFast</t>
   </si>
 </sst>
 </file>
@@ -375,7 +381,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +407,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -409,7 +415,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -417,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -425,7 +431,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -436,10 +442,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -447,10 +453,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -458,10 +464,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -469,10 +475,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -480,7 +486,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
@@ -491,10 +497,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -502,10 +508,10 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -513,10 +519,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -524,93 +530,105 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Rename HO_VectorBox and add initial fault
</commit_message>
<xml_diff>
--- a/matlab_code/etc_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/etc_benchTest/CANmailboxUsage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\etc_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D32E32B-9904-4883-BBD4-078F53832004}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991219C5-3A76-42CD-8393-936F6F66B624}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -36,15 +36,9 @@
     <t>Location</t>
   </si>
   <si>
-    <t>HO_VectorBox/motorMeasurements</t>
-  </si>
-  <si>
     <t>CCP</t>
   </si>
   <si>
-    <t>HO_VectorBox/rawInputs</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -54,13 +48,22 @@
     <t>Input</t>
   </si>
   <si>
-    <t>HO_VectorBox/modes</t>
-  </si>
-  <si>
-    <t>HO_VectorBox/motorControlSlow</t>
-  </si>
-  <si>
-    <t>HO_VectorBox/motorControlFast</t>
+    <t>HO_CAN/Faults</t>
+  </si>
+  <si>
+    <t>HO_CAN/motorMeasurements</t>
+  </si>
+  <si>
+    <t>HO_CAN/motorControlSlow</t>
+  </si>
+  <si>
+    <t>HO_CAN/rawInputs</t>
+  </si>
+  <si>
+    <t>HO_CAN/motorControlFast</t>
+  </si>
+  <si>
+    <t>HO_CAN/modes</t>
   </si>
 </sst>
 </file>
@@ -381,7 +384,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +410,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -415,7 +418,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -423,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -431,10 +434,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -442,10 +445,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -453,10 +456,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -464,10 +467,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -475,7 +478,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -486,10 +489,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -497,10 +500,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -508,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -519,10 +522,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -530,10 +533,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -541,10 +544,10 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -552,20 +555,32 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>